<commit_message>
GDE-9498: Initial Commit for Deal Creation
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="2688" windowWidth="23040" windowHeight="6204" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED01_DealSetup" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -139,7 +139,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -214,6 +214,9 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -596,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:CZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -704,8 +707,8 @@
     <col width="12" bestFit="1" customWidth="1" style="18" min="102" max="102"/>
     <col width="17.44140625" bestFit="1" customWidth="1" style="18" min="103" max="103"/>
     <col width="17.77734375" bestFit="1" customWidth="1" style="18" min="104" max="104"/>
-    <col width="9.109375" customWidth="1" style="18" min="105" max="111"/>
-    <col width="9.109375" customWidth="1" style="18" min="112" max="16384"/>
+    <col width="9.109375" customWidth="1" style="18" min="105" max="117"/>
+    <col width="9.109375" customWidth="1" style="18" min="118" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1552,12 +1555,12 @@
       </c>
       <c r="BP2" s="20" t="inlineStr">
         <is>
-          <t>PT Health</t>
+          <t>EL</t>
         </is>
       </c>
       <c r="BQ2" s="20" t="inlineStr">
         <is>
-          <t>Lightfoot, Edward</t>
+          <t>Lightfoot,  Edward</t>
         </is>
       </c>
       <c r="BR2" s="20" t="inlineStr">
@@ -1715,23 +1718,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20">
       <c r="C20" s="18" t="inlineStr">
         <is>
@@ -1775,10 +1761,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1804,22 +1790,30 @@
     <col width="19.33203125" bestFit="1" customWidth="1" style="11" min="19" max="19"/>
     <col width="22.33203125" bestFit="1" customWidth="1" style="11" min="20" max="20"/>
     <col width="19.109375" bestFit="1" customWidth="1" style="11" min="21" max="21"/>
-    <col width="16.33203125" bestFit="1" customWidth="1" style="11" min="22" max="22"/>
-    <col width="18.88671875" bestFit="1" customWidth="1" style="11" min="23" max="23"/>
-    <col width="25" bestFit="1" customWidth="1" style="11" min="24" max="24"/>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="11" min="25" max="25"/>
-    <col width="28.88671875" bestFit="1" customWidth="1" style="11" min="26" max="26"/>
-    <col width="26.6640625" bestFit="1" customWidth="1" style="11" min="27" max="27"/>
-    <col width="36.6640625" bestFit="1" customWidth="1" style="11" min="28" max="28"/>
-    <col width="35.109375" bestFit="1" customWidth="1" style="11" min="29" max="29"/>
-    <col width="17.33203125" bestFit="1" customWidth="1" style="11" min="30" max="30"/>
-    <col width="35.6640625" bestFit="1" customWidth="1" style="11" min="31" max="31"/>
-    <col width="29.6640625" bestFit="1" customWidth="1" style="11" min="32" max="32"/>
-    <col width="25.88671875" bestFit="1" customWidth="1" style="11" min="33" max="33"/>
-    <col width="13.109375" bestFit="1" customWidth="1" style="11" min="34" max="34"/>
-    <col width="11.5546875" bestFit="1" customWidth="1" style="11" min="35" max="35"/>
-    <col width="9.109375" customWidth="1" style="11" min="36" max="46"/>
-    <col width="9.109375" customWidth="1" style="11" min="47" max="16384"/>
+    <col width="19.109375" customWidth="1" style="11" min="22" max="23"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" style="11" min="24" max="24"/>
+    <col width="18.88671875" bestFit="1" customWidth="1" style="11" min="25" max="25"/>
+    <col width="25" bestFit="1" customWidth="1" style="11" min="26" max="26"/>
+    <col width="25" customWidth="1" style="11" min="27" max="27"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="11" min="28" max="28"/>
+    <col width="28.88671875" bestFit="1" customWidth="1" style="11" min="29" max="29"/>
+    <col width="26.6640625" bestFit="1" customWidth="1" style="11" min="30" max="30"/>
+    <col width="36.6640625" bestFit="1" customWidth="1" style="11" min="31" max="31"/>
+    <col width="35.109375" bestFit="1" customWidth="1" style="11" min="32" max="32"/>
+    <col width="17.33203125" bestFit="1" customWidth="1" style="11" min="33" max="33"/>
+    <col width="35.6640625" bestFit="1" customWidth="1" style="11" min="34" max="34"/>
+    <col width="29.6640625" bestFit="1" customWidth="1" style="11" min="35" max="35"/>
+    <col width="25.88671875" bestFit="1" customWidth="1" style="11" min="36" max="36"/>
+    <col width="13.109375" bestFit="1" customWidth="1" style="11" min="37" max="37"/>
+    <col width="11.5546875" bestFit="1" customWidth="1" style="11" min="38" max="38"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="11" min="39" max="39"/>
+    <col width="17" bestFit="1" customWidth="1" style="11" min="40" max="40"/>
+    <col width="25.44140625" bestFit="1" customWidth="1" style="11" min="41" max="41"/>
+    <col width="25.44140625" customWidth="1" style="11" min="42" max="42"/>
+    <col width="37.88671875" bestFit="1" customWidth="1" style="11" min="43" max="43"/>
+    <col width="25.44140625" bestFit="1" customWidth="1" style="11" min="44" max="44"/>
+    <col width="9.109375" customWidth="1" style="11" min="45" max="56"/>
+    <col width="9.109375" customWidth="1" style="11" min="57" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customFormat="1" customHeight="1" s="5">
@@ -1935,67 +1929,112 @@
       </c>
       <c r="W1" s="2" t="inlineStr">
         <is>
+          <t>HolidayCalendar2</t>
+        </is>
+      </c>
+      <c r="X1" s="2" t="inlineStr">
+        <is>
+          <t>HolidayCalendar3</t>
+        </is>
+      </c>
+      <c r="Y1" s="2" t="inlineStr">
+        <is>
           <t>Deal_PricingOption</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="Z1" s="2" t="inlineStr">
         <is>
           <t>InitialFractionRate_Round</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="AA1" s="2" t="inlineStr">
+        <is>
+          <t>RoundingDecimal_Precision</t>
+        </is>
+      </c>
+      <c r="AB1" s="2" t="inlineStr">
         <is>
           <t>RoundingDecimal_Round</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="AC1" s="2" t="inlineStr">
         <is>
           <t>NonBusinessDayRule</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AD1" s="2" t="inlineStr">
         <is>
           <t>PricingOption_BillNoOfDays</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AE1" s="2" t="inlineStr">
         <is>
           <t>PricingOption_MatrixChangeAppMthd</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AF1" s="2" t="inlineStr">
         <is>
           <t>PricingOption_RateChangeAppMthd</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AG1" s="2" t="inlineStr">
         <is>
           <t>PricingRule_Fee1</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AH1" s="2" t="inlineStr">
         <is>
           <t>PricingRule_MatrixChangeAppMthd1</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AI1" s="2" t="inlineStr">
         <is>
           <t>PricingRule_NonBussDayRule1</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AJ1" s="2" t="inlineStr">
         <is>
           <t>PricingRule_BillNoOfDays1</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>ApproveDate</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AL1" s="4" t="inlineStr">
         <is>
           <t>CloseDate</t>
+        </is>
+      </c>
+      <c r="AM1" s="2" t="inlineStr">
+        <is>
+          <t>PricingOption_IntentNoticeTime</t>
+        </is>
+      </c>
+      <c r="AN1" s="2" t="inlineStr">
+        <is>
+          <t>PricingOption_IntentNoticeDay</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="inlineStr">
+        <is>
+          <t>Minimum_Payment_Amount</t>
+        </is>
+      </c>
+      <c r="AP1" s="2" t="inlineStr">
+        <is>
+          <t>PricingOption_InterestDueUponPrincipalPayment</t>
+        </is>
+      </c>
+      <c r="AQ1" s="2" t="inlineStr">
+        <is>
+          <t>PricingOption_InterestDueUponRepricing</t>
+        </is>
+      </c>
+      <c r="AR1" s="2" t="inlineStr">
+        <is>
+          <t>PricingOption_BillBorrower</t>
         </is>
       </c>
     </row>
@@ -2012,22 +2051,22 @@
       </c>
       <c r="C2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND DEAL AUD 500M 23NOV18</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL2011</t>
         </is>
       </c>
       <c r="D2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND_</t>
+          <t>PT HEALTH SYND</t>
         </is>
       </c>
       <c r="E2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND DEAL AUD 500M 23NOV1840109</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201102114</t>
         </is>
       </c>
       <c r="F2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND_40109</t>
+          <t>PT HEALTH SYND02114</t>
         </is>
       </c>
       <c r="G2" s="7" t="inlineStr">
@@ -2057,7 +2096,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+          <t>WESTPACKBANKINGCORP</t>
         </is>
       </c>
       <c r="M2" s="7" t="inlineStr">
@@ -2067,19 +2106,19 @@
       </c>
       <c r="N2" s="7" t="inlineStr">
         <is>
+          <t>LOANS ADMIN</t>
+        </is>
+      </c>
+      <c r="O2" s="7" t="inlineStr">
+        <is>
+          <t>BLACK</t>
+        </is>
+      </c>
+      <c r="P2" s="7" t="inlineStr">
+        <is>
           <t>AGENCY</t>
         </is>
       </c>
-      <c r="O2" s="7" t="inlineStr">
-        <is>
-          <t>AGENCY</t>
-        </is>
-      </c>
-      <c r="P2" s="7" t="inlineStr">
-        <is>
-          <t>AGENCY</t>
-        </is>
-      </c>
       <c r="Q2" s="8" t="inlineStr">
         <is>
           <t>DDA</t>
@@ -2107,72 +2146,109 @@
       </c>
       <c r="V2" s="7" t="inlineStr">
         <is>
+          <t>Adelaide, Australia</t>
+        </is>
+      </c>
+      <c r="W2" s="7" t="inlineStr">
+        <is>
+          <t>Melbourne, Australia</t>
+        </is>
+      </c>
+      <c r="X2" s="7" t="inlineStr">
+        <is>
           <t>Sydney, Australia</t>
         </is>
       </c>
-      <c r="W2" s="7" t="inlineStr">
+      <c r="Y2" s="7" t="inlineStr">
         <is>
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="X2" s="7" t="inlineStr">
+      <c r="Z2" s="7" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="Y2" s="7" t="inlineStr">
-        <is>
-          <t>Actual</t>
-        </is>
-      </c>
-      <c r="Z2" s="6" t="inlineStr">
+      <c r="AA2" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="7" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="AC2" s="6" t="inlineStr">
         <is>
           <t>Modified Following Business Day</t>
         </is>
       </c>
-      <c r="AA2" s="6" t="inlineStr">
+      <c r="AD2" s="6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="AB2" s="6" t="inlineStr">
-        <is>
-          <t>Next repricing date</t>
-        </is>
-      </c>
-      <c r="AC2" s="6" t="inlineStr">
+      <c r="AE2" s="6" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="AF2" s="6" t="inlineStr">
         <is>
           <t>Start of next interest cycle</t>
         </is>
       </c>
-      <c r="AD2" s="6" t="inlineStr">
+      <c r="AG2" s="6" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="AE2" s="6" t="inlineStr">
-        <is>
-          <t>Start of next cycle</t>
-        </is>
-      </c>
-      <c r="AF2" s="6" t="inlineStr">
+      <c r="AH2" s="6" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="AI2" s="6" t="inlineStr">
         <is>
           <t>Modified Following Business Day</t>
         </is>
       </c>
-      <c r="AG2" s="6" t="inlineStr">
+      <c r="AJ2" s="6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="AH2" s="10" t="inlineStr">
+      <c r="AK2" s="10" t="inlineStr">
         <is>
           <t>27-Jul-2011</t>
         </is>
       </c>
-      <c r="AI2" s="10" t="inlineStr">
+      <c r="AL2" s="10" t="inlineStr">
         <is>
           <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="AM2" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="6" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="AP2" s="6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="AQ2" s="6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="AR2" s="6" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-9499: Initial commit for Facility
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
@@ -3,11 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="2688" windowWidth="23040" windowHeight="6204" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-3660" yWindow="4836" windowWidth="23040" windowHeight="6204" tabRatio="600" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED01_DealSetup" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED02_FacilitySetup" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED08_OngoingFeeSetup" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYND02_PrimaryAllocation" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_CommitmentFeePayment" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -19,7 +23,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,8 +81,14 @@
       <charset val="1"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color indexed="8"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -109,6 +119,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.3499862666707358"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -134,12 +150,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -218,11 +235,90 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal 3 2 2" xfId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -599,8 +695,8 @@
   </sheetPr>
   <dimension ref="A1:CZ23"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -707,8 +803,8 @@
     <col width="12" bestFit="1" customWidth="1" style="18" min="102" max="102"/>
     <col width="17.44140625" bestFit="1" customWidth="1" style="18" min="103" max="103"/>
     <col width="17.77734375" bestFit="1" customWidth="1" style="18" min="104" max="104"/>
-    <col width="9.109375" customWidth="1" style="18" min="105" max="117"/>
-    <col width="9.109375" customWidth="1" style="18" min="118" max="16384"/>
+    <col width="9.109375" customWidth="1" style="18" min="105" max="140"/>
+    <col width="9.109375" customWidth="1" style="18" min="141" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1233,7 +1329,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="26.4" customHeight="1">
+    <row r="2" ht="26.4" customHeight="1" s="49">
       <c r="A2" s="19" t="inlineStr">
         <is>
           <t>1</t>
@@ -1763,8 +1859,8 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1812,8 +1908,8 @@
     <col width="25.44140625" customWidth="1" style="11" min="42" max="42"/>
     <col width="37.88671875" bestFit="1" customWidth="1" style="11" min="43" max="43"/>
     <col width="25.44140625" bestFit="1" customWidth="1" style="11" min="44" max="44"/>
-    <col width="9.109375" customWidth="1" style="11" min="45" max="56"/>
-    <col width="9.109375" customWidth="1" style="11" min="57" max="16384"/>
+    <col width="9.109375" customWidth="1" style="11" min="45" max="79"/>
+    <col width="9.109375" customWidth="1" style="11" min="80" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customFormat="1" customHeight="1" s="5">
@@ -2061,12 +2157,12 @@
       </c>
       <c r="E2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND AUD2.5B 27JUL201102114</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
         </is>
       </c>
       <c r="F2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND02114</t>
+          <t>PT HEALTH SYND30115</t>
         </is>
       </c>
       <c r="G2" s="7" t="inlineStr">
@@ -2249,6 +2345,1120 @@
       <c r="AR2" s="6" t="inlineStr">
         <is>
           <t>N</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AX2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="8.88671875" customWidth="1" style="49" min="1" max="1"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" style="49" min="2" max="2"/>
+    <col width="37.109375" bestFit="1" customWidth="1" style="49" min="3" max="3"/>
+    <col width="42.44140625" bestFit="1" customWidth="1" style="49" min="4" max="4"/>
+    <col width="14" bestFit="1" customWidth="1" style="49" min="5" max="5"/>
+    <col width="13.109375" bestFit="1" customWidth="1" style="49" min="6" max="6"/>
+    <col width="24.6640625" bestFit="1" customWidth="1" style="49" min="7" max="7"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="49" min="8" max="8"/>
+    <col width="23.109375" bestFit="1" customWidth="1" style="49" min="9" max="9"/>
+    <col width="20.6640625" bestFit="1" customWidth="1" style="49" min="10" max="10"/>
+    <col width="18.6640625" bestFit="1" customWidth="1" style="49" min="11" max="11"/>
+    <col width="20.33203125" bestFit="1" customWidth="1" style="49" min="12" max="12"/>
+    <col width="23.109375" bestFit="1" customWidth="1" style="49" min="13" max="13"/>
+    <col width="36.33203125" bestFit="1" customWidth="1" style="49" min="14" max="14"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="49" min="15" max="15"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" style="49" min="16" max="16"/>
+    <col width="48" bestFit="1" customWidth="1" style="49" min="17" max="17"/>
+    <col width="19.44140625" bestFit="1" customWidth="1" style="49" min="18" max="18"/>
+    <col width="32" bestFit="1" customWidth="1" style="49" min="19" max="19"/>
+    <col width="19.44140625" bestFit="1" customWidth="1" style="49" min="20" max="20"/>
+    <col width="22.5546875" bestFit="1" customWidth="1" style="49" min="21" max="21"/>
+    <col width="25.5546875" bestFit="1" customWidth="1" style="49" min="22" max="22"/>
+    <col width="24.44140625" bestFit="1" customWidth="1" style="49" min="23" max="23"/>
+    <col width="24.6640625" bestFit="1" customWidth="1" style="49" min="24" max="24"/>
+    <col width="14.44140625" bestFit="1" customWidth="1" style="49" min="25" max="25"/>
+    <col width="18.33203125" bestFit="1" customWidth="1" style="49" min="26" max="26"/>
+    <col width="8.88671875" customWidth="1" style="49" min="27" max="48"/>
+    <col width="8.88671875" customWidth="1" style="49" min="49" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.2" customFormat="1" customHeight="1" s="47">
+      <c r="A1" s="45" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="45" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="45" t="inlineStr">
+        <is>
+          <t>Facility_NamePrefix</t>
+        </is>
+      </c>
+      <c r="D1" s="46" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="46" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="F1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_Type</t>
+        </is>
+      </c>
+      <c r="G1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_ProposedCmtAmt</t>
+        </is>
+      </c>
+      <c r="H1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_Currency</t>
+        </is>
+      </c>
+      <c r="I1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_AgreementDate</t>
+        </is>
+      </c>
+      <c r="J1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="K1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_ExpiryDate</t>
+        </is>
+      </c>
+      <c r="L1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_MaturityDate</t>
+        </is>
+      </c>
+      <c r="M1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_ServicingGroup</t>
+        </is>
+      </c>
+      <c r="N1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_Customer</t>
+        </is>
+      </c>
+      <c r="O1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_RiskType</t>
+        </is>
+      </c>
+      <c r="P1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_RiskTypeLimit</t>
+        </is>
+      </c>
+      <c r="Q1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_LoanPurposeType</t>
+        </is>
+      </c>
+      <c r="R1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_GlobalLimit</t>
+        </is>
+      </c>
+      <c r="S1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_CustomerServicingGroup</t>
+        </is>
+      </c>
+      <c r="T1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_SGLocation</t>
+        </is>
+      </c>
+      <c r="U1" s="46" t="inlineStr">
+        <is>
+          <t>Facility_Borrower</t>
+        </is>
+      </c>
+      <c r="V1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerSGName</t>
+        </is>
+      </c>
+      <c r="W1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerPercent</t>
+        </is>
+      </c>
+      <c r="X1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerMaturity</t>
+        </is>
+      </c>
+      <c r="Y1" s="47" t="inlineStr">
+        <is>
+          <t>Deal_Currency</t>
+        </is>
+      </c>
+      <c r="Z1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_Borrower1</t>
+        </is>
+      </c>
+      <c r="AA1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_Borrower2</t>
+        </is>
+      </c>
+      <c r="AB1" s="47" t="inlineStr">
+        <is>
+          <t>Borrower_Currency1</t>
+        </is>
+      </c>
+      <c r="AC1" s="47" t="inlineStr">
+        <is>
+          <t>Borrower_Currency2</t>
+        </is>
+      </c>
+      <c r="AD1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerMaturity2</t>
+        </is>
+      </c>
+      <c r="AE1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerSGName2</t>
+        </is>
+      </c>
+      <c r="AF1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_BorrowerPercent2</t>
+        </is>
+      </c>
+      <c r="AG1" s="47" t="inlineStr">
+        <is>
+          <t>SublimitCust_EffectiveDate1</t>
+        </is>
+      </c>
+      <c r="AH1" s="47" t="inlineStr">
+        <is>
+          <t>SublimitCust_EffectiveDate2</t>
+        </is>
+      </c>
+      <c r="AI1" s="47" t="inlineStr">
+        <is>
+          <t>CurrencyLimit1</t>
+        </is>
+      </c>
+      <c r="AJ1" s="47" t="inlineStr">
+        <is>
+          <t>CurrencyLimit2</t>
+        </is>
+      </c>
+      <c r="AK1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_GlobalLimit1</t>
+        </is>
+      </c>
+      <c r="AL1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_GlobalLimit2</t>
+        </is>
+      </c>
+      <c r="AM1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_CustomerServicingGroup1</t>
+        </is>
+      </c>
+      <c r="AN1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_CustomerServicingGroup2</t>
+        </is>
+      </c>
+      <c r="AO1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_SGAlias1</t>
+        </is>
+      </c>
+      <c r="AP1" s="47" t="inlineStr">
+        <is>
+          <t>Facility_SGAlias2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="44">
+      <c r="A2" s="36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>Establish Syndicated Deal</t>
+        </is>
+      </c>
+      <c r="C2" s="37" t="inlineStr">
+        <is>
+          <t>TERM FACILITY</t>
+        </is>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+        </is>
+      </c>
+      <c r="E2" s="37" t="inlineStr">
+        <is>
+          <t>TERM FACILITY36140</t>
+        </is>
+      </c>
+      <c r="F2" s="36" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="G2" s="38" t="inlineStr">
+        <is>
+          <t>2,287,051,025.04</t>
+        </is>
+      </c>
+      <c r="H2" s="36" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="I2" s="39" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="J2" s="39" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="K2" s="39" t="inlineStr">
+        <is>
+          <t>05-Sep-2020</t>
+        </is>
+      </c>
+      <c r="L2" s="39" t="inlineStr">
+        <is>
+          <t>05-Sep-2020</t>
+        </is>
+      </c>
+      <c r="M2" s="37" t="inlineStr">
+        <is>
+          <t>NON AGENCY</t>
+        </is>
+      </c>
+      <c r="N2" s="40" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="O2" s="38" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="P2" s="38" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="Q2" s="36" t="inlineStr">
+        <is>
+          <t>Refinance of existing loan from Other Financial institution</t>
+        </is>
+      </c>
+      <c r="R2" s="36" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="S2" s="41" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="T2" s="36" t="n"/>
+      <c r="U2" s="20" t="inlineStr">
+        <is>
+          <t>VIRUS SLAYERS LTD 1515557</t>
+        </is>
+      </c>
+      <c r="V2" s="36" t="inlineStr">
+        <is>
+          <t>LIGHTFOOT</t>
+        </is>
+      </c>
+      <c r="W2" s="36" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="X2" s="36" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="Y2" s="42" t="n"/>
+      <c r="Z2" s="43" t="n"/>
+      <c r="AG2" s="48" t="n"/>
+      <c r="AH2" s="48" t="n"/>
+      <c r="AQ2" s="43" t="n"/>
+      <c r="AR2" s="43" t="n"/>
+      <c r="AS2" s="43" t="n"/>
+      <c r="AT2" s="43" t="n"/>
+      <c r="AU2" s="43" t="n"/>
+      <c r="AV2" s="43" t="n"/>
+      <c r="AW2" s="43" t="n"/>
+      <c r="AX2" s="43" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="6.109375" bestFit="1" customWidth="1" style="53" min="1" max="1"/>
+    <col width="20.109375" bestFit="1" customWidth="1" style="53" min="2" max="2"/>
+    <col width="15.5546875" bestFit="1" customWidth="1" style="53" min="3" max="3"/>
+    <col width="14.5546875" bestFit="1" customWidth="1" style="53" min="4" max="4"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" style="53" min="5" max="5"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="53" min="6" max="6"/>
+    <col width="22.44140625" bestFit="1" customWidth="1" style="53" min="7" max="7"/>
+    <col width="16" bestFit="1" customWidth="1" style="53" min="8" max="8"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" style="53" min="9" max="9"/>
+    <col width="19.6640625" bestFit="1" customWidth="1" style="53" min="10" max="10"/>
+    <col width="16.6640625" bestFit="1" customWidth="1" style="53" min="11" max="11"/>
+    <col width="18.44140625" bestFit="1" customWidth="1" style="53" min="12" max="12"/>
+    <col width="12.33203125" bestFit="1" customWidth="1" style="53" min="13" max="13"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="53" min="14" max="14"/>
+    <col width="9.21875" bestFit="1" customWidth="1" style="53" min="15" max="15"/>
+    <col width="18" bestFit="1" customWidth="1" style="53" min="16" max="16"/>
+    <col width="6.109375" bestFit="1" customWidth="1" style="53" min="17" max="17"/>
+    <col width="10.44140625" customWidth="1" style="53" min="18" max="34"/>
+    <col width="10.44140625" customWidth="1" style="53" min="35" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="50" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="51" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="52" t="inlineStr">
+        <is>
+          <t>Penalty_Spread</t>
+        </is>
+      </c>
+      <c r="D1" s="52" t="inlineStr">
+        <is>
+          <t>Penalty_Status</t>
+        </is>
+      </c>
+      <c r="E1" s="51" t="inlineStr">
+        <is>
+          <t>OngoingFee_Category</t>
+        </is>
+      </c>
+      <c r="F1" s="51" t="inlineStr">
+        <is>
+          <t>OngoingFee_Type</t>
+        </is>
+      </c>
+      <c r="G1" s="51" t="inlineStr">
+        <is>
+          <t>OngoingFee_RateBasis</t>
+        </is>
+      </c>
+      <c r="H1" s="51" t="inlineStr">
+        <is>
+          <t>FacilityItemAfter</t>
+        </is>
+      </c>
+      <c r="I1" s="51" t="inlineStr">
+        <is>
+          <t>Facility_PercentWhole1</t>
+        </is>
+      </c>
+      <c r="J1" s="51" t="inlineStr">
+        <is>
+          <t>FacilityItem</t>
+        </is>
+      </c>
+      <c r="K1" s="51" t="inlineStr">
+        <is>
+          <t>Facility_Percent1</t>
+        </is>
+      </c>
+      <c r="L1" s="51" t="inlineStr">
+        <is>
+          <t>InterestPricingItem</t>
+        </is>
+      </c>
+      <c r="M1" s="51" t="inlineStr">
+        <is>
+          <t>OptionName</t>
+        </is>
+      </c>
+      <c r="N1" s="51" t="inlineStr">
+        <is>
+          <t>Interest_RateBasis</t>
+        </is>
+      </c>
+      <c r="O1" s="51" t="inlineStr">
+        <is>
+          <t>Spread1</t>
+        </is>
+      </c>
+      <c r="P1" s="51" t="inlineStr">
+        <is>
+          <t>FormulaText</t>
+        </is>
+      </c>
+      <c r="Q1" s="51" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="55" t="inlineStr">
+        <is>
+          <t>Establish Ongoing Fee</t>
+        </is>
+      </c>
+      <c r="C2" s="56" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="D2" s="57" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="E2" s="22" t="inlineStr">
+        <is>
+          <t>Facility Ongoing Fee</t>
+        </is>
+      </c>
+      <c r="F2" s="22" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="G2" s="22" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="H2" s="20" t="inlineStr">
+        <is>
+          <t>FormulaCategory</t>
+        </is>
+      </c>
+      <c r="I2" s="58" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J2" s="20" t="inlineStr">
+        <is>
+          <t>Global Current  X Rate</t>
+        </is>
+      </c>
+      <c r="K2" s="58" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="L2" s="58" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="M2" s="58" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="N2" s="58" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="O2" s="58" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="P2" s="58" t="inlineStr">
+        <is>
+          <t>HigherOf(BBSY,0%)</t>
+        </is>
+      </c>
+      <c r="Q2" s="58" t="inlineStr">
+        <is>
+          <t>BBSY</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="6.109375" customWidth="1" style="18" min="1" max="1"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
+    <col width="39.5546875" bestFit="1" customWidth="1" style="18" min="3" max="3"/>
+    <col width="31.88671875" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
+    <col width="12.88671875" bestFit="1" customWidth="1" style="18" min="5" max="5"/>
+    <col width="13.6640625" bestFit="1" customWidth="1" style="18" min="6" max="6"/>
+    <col width="36.33203125" bestFit="1" customWidth="1" style="18" min="7" max="7"/>
+    <col width="21" customWidth="1" style="18" min="8" max="8"/>
+    <col width="24.5546875" customWidth="1" style="65" min="9" max="9"/>
+    <col width="19.44140625" customWidth="1" style="65" min="10" max="11"/>
+    <col width="21.109375" bestFit="1" customWidth="1" style="65" min="12" max="12"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" style="65" min="13" max="13"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="65" min="14" max="14"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" style="65" min="15" max="15"/>
+    <col width="18.88671875" customWidth="1" style="65" min="16" max="16"/>
+    <col width="26.33203125" customWidth="1" style="65" min="17" max="17"/>
+    <col width="34.88671875" customWidth="1" style="65" min="18" max="18"/>
+    <col width="25.5546875" bestFit="1" customWidth="1" style="18" min="19" max="19"/>
+    <col width="26.33203125" customWidth="1" style="18" min="20" max="20"/>
+    <col width="34.88671875" customWidth="1" style="18" min="21" max="21"/>
+    <col width="26.5546875" customWidth="1" style="18" min="22" max="22"/>
+    <col width="27.33203125" customWidth="1" style="18" min="23" max="23"/>
+    <col width="20" customWidth="1" style="18" min="24" max="24"/>
+    <col width="36.109375" customWidth="1" style="18" min="25" max="25"/>
+    <col width="18.109375" customWidth="1" style="18" min="26" max="26"/>
+    <col width="12.6640625" customWidth="1" style="67" min="27" max="27"/>
+    <col width="11.109375" bestFit="1" customWidth="1" style="67" min="28" max="28"/>
+    <col width="23" bestFit="1" customWidth="1" style="18" min="29" max="29"/>
+    <col width="18.88671875" bestFit="1" customWidth="1" style="18" min="30" max="30"/>
+    <col width="9.109375" customWidth="1" style="53" min="31" max="42"/>
+    <col width="9.109375" customWidth="1" style="53" min="43" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.2" customFormat="1" customHeight="1" s="60">
+      <c r="A1" s="12" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="13" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="15" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="15" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="14" t="inlineStr">
+        <is>
+          <t>LenderType1</t>
+        </is>
+      </c>
+      <c r="F1" s="14" t="inlineStr">
+        <is>
+          <t>LenderType2</t>
+        </is>
+      </c>
+      <c r="G1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_Lender1</t>
+        </is>
+      </c>
+      <c r="H1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_LenderLoc1</t>
+        </is>
+      </c>
+      <c r="I1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_TransactionType</t>
+        </is>
+      </c>
+      <c r="J1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_PctOfDeal1</t>
+        </is>
+      </c>
+      <c r="K1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_PctOfDeal2</t>
+        </is>
+      </c>
+      <c r="L1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_BuySellPrice</t>
+        </is>
+      </c>
+      <c r="M1" s="59" t="inlineStr">
+        <is>
+          <t>Expected_CloseDate</t>
+        </is>
+      </c>
+      <c r="N1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_Contact1</t>
+        </is>
+      </c>
+      <c r="O1" s="59" t="inlineStr">
+        <is>
+          <t>AdminAgent_SGAlias1</t>
+        </is>
+      </c>
+      <c r="P1" s="59" t="inlineStr">
+        <is>
+          <t>Deal_ExpenseCode</t>
+        </is>
+      </c>
+      <c r="Q1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_Portfolio</t>
+        </is>
+      </c>
+      <c r="R1" s="59" t="inlineStr">
+        <is>
+          <t>Primary_PortfolioBranch</t>
+        </is>
+      </c>
+      <c r="S1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_RiskBook</t>
+        </is>
+      </c>
+      <c r="T1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_Portfolio</t>
+        </is>
+      </c>
+      <c r="U1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_PortfolioBranch</t>
+        </is>
+      </c>
+      <c r="V1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_PortfolioAllocation</t>
+        </is>
+      </c>
+      <c r="W1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_PortfolioExpiryDate</t>
+        </is>
+      </c>
+      <c r="X1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_CircledDate</t>
+        </is>
+      </c>
+      <c r="Y1" s="13" t="inlineStr">
+        <is>
+          <t>PortfolioBranch</t>
+        </is>
+      </c>
+      <c r="Z1" s="13" t="inlineStr">
+        <is>
+          <t>PortfolioAllocation</t>
+        </is>
+      </c>
+      <c r="AA1" s="13" t="inlineStr">
+        <is>
+          <t>ApproveDate</t>
+        </is>
+      </c>
+      <c r="AB1" s="13" t="inlineStr">
+        <is>
+          <t>CloseDate</t>
+        </is>
+      </c>
+      <c r="AC1" s="13" t="inlineStr">
+        <is>
+          <t>ServicingGroupMember</t>
+        </is>
+      </c>
+      <c r="AD1" s="13" t="inlineStr">
+        <is>
+          <t>IsLenderAHostBank</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="18">
+      <c r="A2" s="20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="20" t="inlineStr">
+        <is>
+          <t>Establish Primaries</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+        </is>
+      </c>
+      <c r="D2" s="37" t="inlineStr">
+        <is>
+          <t>TERM FACILITY36140</t>
+        </is>
+      </c>
+      <c r="E2" s="61" t="inlineStr">
+        <is>
+          <t>Host Bank</t>
+        </is>
+      </c>
+      <c r="F2" s="61" t="inlineStr">
+        <is>
+          <t>Non-Host Bank</t>
+        </is>
+      </c>
+      <c r="G2" s="20" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="H2" s="22" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="I2" s="22" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="J2" s="22" t="inlineStr">
+        <is>
+          <t>6.27</t>
+        </is>
+      </c>
+      <c r="K2" s="22" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="L2" s="22" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M2" s="62" t="inlineStr">
+        <is>
+          <t>26-Nov-2018</t>
+        </is>
+      </c>
+      <c r="N2" s="22" t="inlineStr">
+        <is>
+          <t>NON AGENCY,  Lending and Leasing</t>
+        </is>
+      </c>
+      <c r="O2" s="63" t="inlineStr">
+        <is>
+          <t>NON AGENCY</t>
+        </is>
+      </c>
+      <c r="P2" s="22" t="inlineStr">
+        <is>
+          <t>RE_PRF</t>
+        </is>
+      </c>
+      <c r="Q2" s="22" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="R2" s="22" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="S2" s="22" t="inlineStr">
+        <is>
+          <t>RE_PRF</t>
+        </is>
+      </c>
+      <c r="T2" s="22" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="U2" s="22" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="V2" s="62" t="inlineStr">
+        <is>
+          <t>143,398,099.27</t>
+        </is>
+      </c>
+      <c r="W2" s="64" t="inlineStr">
+        <is>
+          <t>25-Oct-2023</t>
+        </is>
+      </c>
+      <c r="X2" s="64" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="Y2" s="63" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia -DBU</t>
+        </is>
+      </c>
+      <c r="Z2" s="63" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="AA2" s="64" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="AB2" s="64" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
+      <c r="AC2" s="63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AD2" s="63" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="N3" s="66" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="19.33203125" bestFit="1" customWidth="1" style="49" min="2" max="2"/>
+    <col width="41.5546875" bestFit="1" customWidth="1" style="49" min="3" max="3"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="49" min="4" max="4"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="49" min="5" max="5"/>
+    <col width="24.77734375" bestFit="1" customWidth="1" style="49" min="6" max="6"/>
+    <col width="22.77734375" bestFit="1" customWidth="1" style="49" min="7" max="7"/>
+    <col width="28.5546875" bestFit="1" customWidth="1" style="49" min="8" max="8"/>
+    <col width="19.33203125" bestFit="1" customWidth="1" style="49" min="9" max="9"/>
+    <col width="27.44140625" bestFit="1" customWidth="1" style="49" min="10" max="11"/>
+    <col width="14.77734375" bestFit="1" customWidth="1" style="49" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="68">
+      <c r="A1" s="68" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="68" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="69" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="68" t="inlineStr">
+        <is>
+          <t>OngoingFee_Type</t>
+        </is>
+      </c>
+      <c r="E1" s="69" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="F1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="G1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_ActualDate</t>
+        </is>
+      </c>
+      <c r="H1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_AdjustedDueDate</t>
+        </is>
+      </c>
+      <c r="I1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_Accrue</t>
+        </is>
+      </c>
+      <c r="J1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_AccrualEndDate</t>
+        </is>
+      </c>
+      <c r="K1" s="68" t="inlineStr">
+        <is>
+          <t>Commitment_CycleFrequency</t>
+        </is>
+      </c>
+      <c r="L1" s="68" t="inlineStr">
+        <is>
+          <t>Fee_ExpiryDate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customFormat="1" customHeight="1" s="36">
+      <c r="A2" s="36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="37" t="inlineStr">
+        <is>
+          <t>Deal_New_Life_BILAT</t>
+        </is>
+      </c>
+      <c r="C2" s="37" t="inlineStr">
+        <is>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+        </is>
+      </c>
+      <c r="D2" s="36" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="E2" s="37" t="inlineStr">
+        <is>
+          <t>TERM FACILITY36140</t>
+        </is>
+      </c>
+      <c r="F2" s="39" t="inlineStr">
+        <is>
+          <t>25-Nov-2019</t>
+        </is>
+      </c>
+      <c r="G2" s="39" t="inlineStr">
+        <is>
+          <t>25-Feb-2020</t>
+        </is>
+      </c>
+      <c r="H2" s="39" t="inlineStr">
+        <is>
+          <t>25-Nov-2019</t>
+        </is>
+      </c>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="J2" s="39" t="inlineStr">
+        <is>
+          <t>24-Feb-2020</t>
+        </is>
+      </c>
+      <c r="K2" s="39" t="inlineStr">
+        <is>
+          <t>Quarterly</t>
+        </is>
+      </c>
+      <c r="L2" s="36" t="inlineStr">
+        <is>
+          <t>05-Jun-2020</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-9499: Address Comments to adjust the data and steps
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-3660" yWindow="4836" windowWidth="23040" windowHeight="6204" tabRatio="600" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -803,8 +803,8 @@
     <col width="12" bestFit="1" customWidth="1" style="18" min="102" max="102"/>
     <col width="17.44140625" bestFit="1" customWidth="1" style="18" min="103" max="103"/>
     <col width="17.77734375" bestFit="1" customWidth="1" style="18" min="104" max="104"/>
-    <col width="9.109375" customWidth="1" style="18" min="105" max="140"/>
-    <col width="9.109375" customWidth="1" style="18" min="141" max="16384"/>
+    <col width="9.109375" customWidth="1" style="18" min="105" max="145"/>
+    <col width="9.109375" customWidth="1" style="18" min="146" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1859,8 +1859,8 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1908,8 +1908,10 @@
     <col width="25.44140625" customWidth="1" style="11" min="42" max="42"/>
     <col width="37.88671875" bestFit="1" customWidth="1" style="11" min="43" max="43"/>
     <col width="25.44140625" bestFit="1" customWidth="1" style="11" min="44" max="44"/>
-    <col width="9.109375" customWidth="1" style="11" min="45" max="79"/>
-    <col width="9.109375" customWidth="1" style="11" min="80" max="16384"/>
+    <col width="13.44140625" bestFit="1" customWidth="1" style="11" min="45" max="45"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" style="11" min="46" max="46"/>
+    <col width="9.109375" customWidth="1" style="11" min="47" max="84"/>
+    <col width="9.109375" customWidth="1" style="11" min="85" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customFormat="1" customHeight="1" s="5">
@@ -2157,12 +2159,12 @@
       </c>
       <c r="E2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201139127</t>
         </is>
       </c>
       <c r="F2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND30115</t>
+          <t>PT HEALTH SYND39127</t>
         </is>
       </c>
       <c r="G2" s="7" t="inlineStr">
@@ -2192,7 +2194,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>WESTPACKBANKINGCORP</t>
+          <t>ANZ</t>
         </is>
       </c>
       <c r="M2" s="7" t="inlineStr">
@@ -2202,12 +2204,12 @@
       </c>
       <c r="N2" s="7" t="inlineStr">
         <is>
-          <t>LOANS ADMIN</t>
+          <t>LAD/MG</t>
         </is>
       </c>
       <c r="O2" s="7" t="inlineStr">
         <is>
-          <t>BLACK</t>
+          <t>DORE/GALING</t>
         </is>
       </c>
       <c r="P2" s="7" t="inlineStr">
@@ -2361,8 +2363,8 @@
   </sheetPr>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2393,8 +2395,8 @@
     <col width="24.6640625" bestFit="1" customWidth="1" style="49" min="24" max="24"/>
     <col width="14.44140625" bestFit="1" customWidth="1" style="49" min="25" max="25"/>
     <col width="18.33203125" bestFit="1" customWidth="1" style="49" min="26" max="26"/>
-    <col width="8.88671875" customWidth="1" style="49" min="27" max="48"/>
-    <col width="8.88671875" customWidth="1" style="49" min="49" max="16384"/>
+    <col width="8.88671875" customWidth="1" style="49" min="27" max="53"/>
+    <col width="8.88671875" customWidth="1" style="49" min="54" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customFormat="1" customHeight="1" s="47">
@@ -2622,17 +2624,17 @@
       </c>
       <c r="C2" s="37" t="inlineStr">
         <is>
-          <t>TERM FACILITY</t>
+          <t>CONSTRUCTION TERM FACILITY</t>
         </is>
       </c>
       <c r="D2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201139127</t>
         </is>
       </c>
       <c r="E2" s="37" t="inlineStr">
         <is>
-          <t>TERM FACILITY36140</t>
+          <t>CONSTRUCTION TERM FACILITY4601</t>
         </is>
       </c>
       <c r="F2" s="36" t="inlineStr">
@@ -2754,7 +2756,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.44140625" defaultRowHeight="14.4"/>
@@ -2776,8 +2778,8 @@
     <col width="9.21875" bestFit="1" customWidth="1" style="53" min="15" max="15"/>
     <col width="18" bestFit="1" customWidth="1" style="53" min="16" max="16"/>
     <col width="6.109375" bestFit="1" customWidth="1" style="53" min="17" max="17"/>
-    <col width="10.44140625" customWidth="1" style="53" min="18" max="34"/>
-    <col width="10.44140625" customWidth="1" style="53" min="35" max="16384"/>
+    <col width="10.44140625" customWidth="1" style="53" min="18" max="39"/>
+    <col width="10.44140625" customWidth="1" style="53" min="40" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2959,10 +2961,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2976,28 +2978,29 @@
     <col width="36.33203125" bestFit="1" customWidth="1" style="18" min="7" max="7"/>
     <col width="21" customWidth="1" style="18" min="8" max="8"/>
     <col width="24.5546875" customWidth="1" style="65" min="9" max="9"/>
-    <col width="19.44140625" customWidth="1" style="65" min="10" max="11"/>
-    <col width="21.109375" bestFit="1" customWidth="1" style="65" min="12" max="12"/>
-    <col width="19.88671875" bestFit="1" customWidth="1" style="65" min="13" max="13"/>
-    <col width="28.109375" bestFit="1" customWidth="1" style="65" min="14" max="14"/>
-    <col width="21.6640625" bestFit="1" customWidth="1" style="65" min="15" max="15"/>
-    <col width="18.88671875" customWidth="1" style="65" min="16" max="16"/>
-    <col width="26.33203125" customWidth="1" style="65" min="17" max="17"/>
-    <col width="34.88671875" customWidth="1" style="65" min="18" max="18"/>
-    <col width="25.5546875" bestFit="1" customWidth="1" style="18" min="19" max="19"/>
-    <col width="26.33203125" customWidth="1" style="18" min="20" max="20"/>
-    <col width="34.88671875" customWidth="1" style="18" min="21" max="21"/>
-    <col width="26.5546875" customWidth="1" style="18" min="22" max="22"/>
-    <col width="27.33203125" customWidth="1" style="18" min="23" max="23"/>
-    <col width="20" customWidth="1" style="18" min="24" max="24"/>
-    <col width="36.109375" customWidth="1" style="18" min="25" max="25"/>
-    <col width="18.109375" customWidth="1" style="18" min="26" max="26"/>
-    <col width="12.6640625" customWidth="1" style="67" min="27" max="27"/>
-    <col width="11.109375" bestFit="1" customWidth="1" style="67" min="28" max="28"/>
-    <col width="23" bestFit="1" customWidth="1" style="18" min="29" max="29"/>
-    <col width="18.88671875" bestFit="1" customWidth="1" style="18" min="30" max="30"/>
-    <col width="9.109375" customWidth="1" style="53" min="31" max="42"/>
-    <col width="9.109375" customWidth="1" style="53" min="43" max="16384"/>
+    <col width="19.44140625" customWidth="1" style="65" min="10" max="10"/>
+    <col width="21.109375" bestFit="1" customWidth="1" style="65" min="11" max="11"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" style="65" min="12" max="12"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="65" min="13" max="13"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" style="65" min="14" max="14"/>
+    <col width="18.88671875" customWidth="1" style="65" min="15" max="15"/>
+    <col width="26.33203125" customWidth="1" style="65" min="16" max="16"/>
+    <col width="34.88671875" customWidth="1" style="65" min="17" max="17"/>
+    <col width="25.5546875" bestFit="1" customWidth="1" style="18" min="18" max="18"/>
+    <col width="26.33203125" customWidth="1" style="18" min="19" max="19"/>
+    <col width="34.88671875" customWidth="1" style="18" min="20" max="20"/>
+    <col width="26.5546875" customWidth="1" style="18" min="21" max="21"/>
+    <col width="27.33203125" customWidth="1" style="18" min="22" max="22"/>
+    <col width="20" customWidth="1" style="18" min="23" max="23"/>
+    <col width="36.109375" customWidth="1" style="18" min="24" max="24"/>
+    <col width="18.109375" customWidth="1" style="18" min="25" max="25"/>
+    <col width="12.6640625" customWidth="1" style="67" min="26" max="26"/>
+    <col width="11.109375" bestFit="1" customWidth="1" style="67" min="27" max="27"/>
+    <col width="23" bestFit="1" customWidth="1" style="18" min="28" max="28"/>
+    <col width="18.88671875" bestFit="1" customWidth="1" style="18" min="29" max="29"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" style="53" min="30" max="30"/>
+    <col width="9.109375" customWidth="1" style="53" min="31" max="46"/>
+    <col width="9.109375" customWidth="1" style="53" min="47" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customFormat="1" customHeight="1" s="60">
@@ -3053,102 +3056,107 @@
       </c>
       <c r="K1" s="59" t="inlineStr">
         <is>
-          <t>Primary_PctOfDeal2</t>
+          <t>Primary_BuySellPrice</t>
         </is>
       </c>
       <c r="L1" s="59" t="inlineStr">
         <is>
-          <t>Primary_BuySellPrice</t>
+          <t>Expected_CloseDate</t>
         </is>
       </c>
       <c r="M1" s="59" t="inlineStr">
         <is>
-          <t>Expected_CloseDate</t>
+          <t>Primary_Contact1</t>
         </is>
       </c>
       <c r="N1" s="59" t="inlineStr">
         <is>
-          <t>Primary_Contact1</t>
+          <t>AdminAgent_SGAlias1</t>
         </is>
       </c>
       <c r="O1" s="59" t="inlineStr">
         <is>
-          <t>AdminAgent_SGAlias1</t>
+          <t>Deal_ExpenseCode</t>
         </is>
       </c>
       <c r="P1" s="59" t="inlineStr">
         <is>
-          <t>Deal_ExpenseCode</t>
+          <t>Primary_Portfolio</t>
         </is>
       </c>
       <c r="Q1" s="59" t="inlineStr">
         <is>
+          <t>Primary_PortfolioBranch</t>
+        </is>
+      </c>
+      <c r="R1" s="14" t="inlineStr">
+        <is>
+          <t>Primary_RiskBook</t>
+        </is>
+      </c>
+      <c r="S1" s="14" t="inlineStr">
+        <is>
           <t>Primary_Portfolio</t>
         </is>
       </c>
-      <c r="R1" s="59" t="inlineStr">
+      <c r="T1" s="14" t="inlineStr">
         <is>
           <t>Primary_PortfolioBranch</t>
         </is>
       </c>
-      <c r="S1" s="14" t="inlineStr">
-        <is>
-          <t>Primary_RiskBook</t>
-        </is>
-      </c>
-      <c r="T1" s="14" t="inlineStr">
-        <is>
-          <t>Primary_Portfolio</t>
-        </is>
-      </c>
       <c r="U1" s="14" t="inlineStr">
         <is>
-          <t>Primary_PortfolioBranch</t>
+          <t>Primary_PortfolioAllocation</t>
         </is>
       </c>
       <c r="V1" s="14" t="inlineStr">
         <is>
-          <t>Primary_PortfolioAllocation</t>
+          <t>Primary_PortfolioExpiryDate</t>
         </is>
       </c>
       <c r="W1" s="14" t="inlineStr">
         <is>
-          <t>Primary_PortfolioExpiryDate</t>
-        </is>
-      </c>
-      <c r="X1" s="14" t="inlineStr">
-        <is>
           <t>Primary_CircledDate</t>
         </is>
       </c>
+      <c r="X1" s="13" t="inlineStr">
+        <is>
+          <t>PortfolioBranch</t>
+        </is>
+      </c>
       <c r="Y1" s="13" t="inlineStr">
         <is>
-          <t>PortfolioBranch</t>
+          <t>PortfolioAllocation</t>
         </is>
       </c>
       <c r="Z1" s="13" t="inlineStr">
         <is>
-          <t>PortfolioAllocation</t>
+          <t>ApproveDate</t>
         </is>
       </c>
       <c r="AA1" s="13" t="inlineStr">
         <is>
-          <t>ApproveDate</t>
+          <t>CloseDate</t>
         </is>
       </c>
       <c r="AB1" s="13" t="inlineStr">
         <is>
-          <t>CloseDate</t>
+          <t>ServicingGroupMember</t>
         </is>
       </c>
       <c r="AC1" s="13" t="inlineStr">
         <is>
-          <t>ServicingGroupMember</t>
+          <t>IsLenderAHostBank</t>
         </is>
       </c>
       <c r="AD1" s="13" t="inlineStr">
         <is>
-          <t>IsLenderAHostBank</t>
+          <t>RunTimeVar_SellAmount</t>
+        </is>
+      </c>
+      <c r="AE1" s="13" t="inlineStr">
+        <is>
+          <t>Precision</t>
         </is>
       </c>
     </row>
@@ -3165,12 +3173,12 @@
       </c>
       <c r="C2" s="7" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201139127</t>
         </is>
       </c>
       <c r="D2" s="37" t="inlineStr">
         <is>
-          <t>TERM FACILITY36140</t>
+          <t>CONSTRUCTION TERM FACILITY4601</t>
         </is>
       </c>
       <c r="E2" s="61" t="inlineStr">
@@ -3200,112 +3208,115 @@
       </c>
       <c r="J2" s="22" t="inlineStr">
         <is>
-          <t>6.27</t>
+          <t xml:space="preserve">6.272875571173 </t>
         </is>
       </c>
       <c r="K2" s="22" t="inlineStr">
         <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="L2" s="22" t="inlineStr">
-        <is>
           <t>100</t>
         </is>
       </c>
-      <c r="M2" s="62" t="inlineStr">
+      <c r="L2" s="62" t="inlineStr">
         <is>
           <t>26-Nov-2018</t>
         </is>
       </c>
-      <c r="N2" s="22" t="inlineStr">
+      <c r="M2" s="22" t="inlineStr">
         <is>
           <t>NON AGENCY,  Lending and Leasing</t>
         </is>
       </c>
-      <c r="O2" s="63" t="inlineStr">
+      <c r="N2" s="63" t="inlineStr">
         <is>
           <t>NON AGENCY</t>
         </is>
       </c>
+      <c r="O2" s="22" t="inlineStr">
+        <is>
+          <t>RE_PRF</t>
+        </is>
+      </c>
       <c r="P2" s="22" t="inlineStr">
         <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="Q2" s="22" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="R2" s="22" t="inlineStr">
+        <is>
           <t>RE_PRF</t>
         </is>
       </c>
-      <c r="Q2" s="22" t="inlineStr">
+      <c r="S2" s="22" t="inlineStr">
         <is>
           <t>Hold for Investment - Australia</t>
         </is>
       </c>
-      <c r="R2" s="22" t="inlineStr">
+      <c r="T2" s="22" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="S2" s="22" t="inlineStr">
-        <is>
-          <t>RE_PRF</t>
-        </is>
-      </c>
-      <c r="T2" s="22" t="inlineStr">
-        <is>
-          <t>Hold for Investment - Australia</t>
-        </is>
-      </c>
-      <c r="U2" s="22" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - DBU</t>
-        </is>
-      </c>
-      <c r="V2" s="62" t="inlineStr">
-        <is>
-          <t>143,398,099.27</t>
+      <c r="U2" s="62" t="inlineStr">
+        <is>
+          <t>143,463,865.05</t>
+        </is>
+      </c>
+      <c r="V2" s="64" t="inlineStr">
+        <is>
+          <t>31-Oct-2023</t>
         </is>
       </c>
       <c r="W2" s="64" t="inlineStr">
         <is>
-          <t>25-Oct-2023</t>
-        </is>
-      </c>
-      <c r="X2" s="64" t="inlineStr">
-        <is>
           <t>27-Jul-2011</t>
         </is>
       </c>
+      <c r="X2" s="63" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia -DBU</t>
+        </is>
+      </c>
       <c r="Y2" s="63" t="inlineStr">
         <is>
-          <t>Commonwealth Bank of Australia -DBU</t>
-        </is>
-      </c>
-      <c r="Z2" s="63" t="inlineStr">
-        <is>
           <t>100,000.00</t>
         </is>
       </c>
+      <c r="Z2" s="64" t="inlineStr">
+        <is>
+          <t>27-Jul-2011</t>
+        </is>
+      </c>
       <c r="AA2" s="64" t="inlineStr">
         <is>
           <t>27-Jul-2011</t>
         </is>
       </c>
-      <c r="AB2" s="64" t="inlineStr">
-        <is>
-          <t>27-Jul-2011</t>
+      <c r="AB2" s="63" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
       <c r="AC2" s="63" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AD2" s="18" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AD2" s="63" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
+      <c r="AE2" s="18" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="N3" s="66" t="n"/>
+      <c r="M3" s="66" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3318,10 +3329,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3336,6 +3347,8 @@
     <col width="19.33203125" bestFit="1" customWidth="1" style="49" min="9" max="9"/>
     <col width="27.44140625" bestFit="1" customWidth="1" style="49" min="10" max="11"/>
     <col width="14.77734375" bestFit="1" customWidth="1" style="49" min="12" max="12"/>
+    <col width="13.44140625" bestFit="1" customWidth="1" style="49" min="13" max="13"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" style="49" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="68">
@@ -3399,6 +3412,16 @@
           <t>Fee_ExpiryDate</t>
         </is>
       </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>FloatRateDate</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>PayType</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15" customFormat="1" customHeight="1" s="36">
       <c r="A2" s="36" t="inlineStr">
@@ -3413,7 +3436,7 @@
       </c>
       <c r="C2" s="37" t="inlineStr">
         <is>
-          <t>PT HEALTH SYND AUD2.5B 27JUL201130115</t>
+          <t>PT HEALTH SYND AUD2.5B 27JUL201139127</t>
         </is>
       </c>
       <c r="D2" s="36" t="inlineStr">
@@ -3423,7 +3446,7 @@
       </c>
       <c r="E2" s="37" t="inlineStr">
         <is>
-          <t>TERM FACILITY36140</t>
+          <t>CONSTRUCTION TERM FACILITY4601</t>
         </is>
       </c>
       <c r="F2" s="39" t="inlineStr">
@@ -3433,7 +3456,7 @@
       </c>
       <c r="G2" s="39" t="inlineStr">
         <is>
-          <t>25-Feb-2020</t>
+          <t>24-Jan-2020</t>
         </is>
       </c>
       <c r="H2" s="39" t="inlineStr">
@@ -3448,7 +3471,7 @@
       </c>
       <c r="J2" s="39" t="inlineStr">
         <is>
-          <t>24-Feb-2020</t>
+          <t>23-Jan-2020</t>
         </is>
       </c>
       <c r="K2" s="39" t="inlineStr">
@@ -3459,6 +3482,16 @@
       <c r="L2" s="36" t="inlineStr">
         <is>
           <t>05-Jun-2020</t>
+        </is>
+      </c>
+      <c r="M2" s="10" t="inlineStr">
+        <is>
+          <t>25-Nov-2019</t>
+        </is>
+      </c>
+      <c r="N2" s="11" t="inlineStr">
+        <is>
+          <t>Pay In Advance</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-9506 - Initial Commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PT_Health_Syndicated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC38283-ECA6-46BC-817F-0A68F1BFBFA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B637CF4-29D6-4327-AD37-C3BE86618765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="SYND02_PrimaryAllocation" sheetId="5" r:id="rId5"/>
     <sheet name="SERV29_CommitmentFeePayment" sheetId="6" r:id="rId6"/>
     <sheet name="SERV01_LoanDrawdown" sheetId="7" r:id="rId7"/>
+    <sheet name="SERV08_ComprehensiveRepricing" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="453">
   <si>
     <t>rowid</t>
   </si>
@@ -1028,6 +1029,9 @@
     <t>563,930.39</t>
   </si>
   <si>
+    <t>-563,930.39</t>
+  </si>
+  <si>
     <t>Establish Ongoing Fee - Period 2</t>
   </si>
   <si>
@@ -1301,7 +1305,88 @@
     <t>3.134300%</t>
   </si>
   <si>
-    <t>-563,930.39</t>
+    <t>OutstandingSelect_Type</t>
+  </si>
+  <si>
+    <t>NewLoan_Alias</t>
+  </si>
+  <si>
+    <t>CombineExistingLoans</t>
+  </si>
+  <si>
+    <t>Delimiter</t>
+  </si>
+  <si>
+    <t>New_LoanAmount</t>
+  </si>
+  <si>
+    <t>Capitalize_PercentOfPayment</t>
+  </si>
+  <si>
+    <t>Repricing_Type</t>
+  </si>
+  <si>
+    <t>Repricing_Add_Option_Setup</t>
+  </si>
+  <si>
+    <t>Repricing_Frequency</t>
+  </si>
+  <si>
+    <t>Base_Rate</t>
+  </si>
+  <si>
+    <t>Cycles_For_Loan</t>
+  </si>
+  <si>
+    <t>Interest_Requested_Amount</t>
+  </si>
+  <si>
+    <t>Expected_LoanCurrentBaseRate</t>
+  </si>
+  <si>
+    <t>Expected_LoanSpread</t>
+  </si>
+  <si>
+    <t>Expected_LoanAllInRate</t>
+  </si>
+  <si>
+    <t>Expected_LoanGlobalOriginal</t>
+  </si>
+  <si>
+    <t>Expected_LoanGlobalCurrent</t>
+  </si>
+  <si>
+    <t>Expected_LoanHostBankGross</t>
+  </si>
+  <si>
+    <t>Expected_LoanHostBankNet</t>
+  </si>
+  <si>
+    <t>21Jan2020_Repricing</t>
+  </si>
+  <si>
+    <t>60003001</t>
+  </si>
+  <si>
+    <t>Comprehensive Repricing</t>
+  </si>
+  <si>
+    <t>Rollover/Conversion to New:</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>0.925000%</t>
+  </si>
+  <si>
+    <t>2,270,856,920.04</t>
+  </si>
+  <si>
+    <t>142,448,028.99</t>
+  </si>
+  <si>
+    <t>3.125000%</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,6 +1472,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1450,7 +1547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1473,6 +1570,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1480,7 +1588,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1682,6 +1790,30 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2109,8 +2241,8 @@
     <col min="102" max="102" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="17.44140625" style="18" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="17.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="105" max="152" width="9.109375" style="18" customWidth="1"/>
-    <col min="153" max="16384" width="9.109375" style="18"/>
+    <col min="105" max="155" width="9.109375" style="18" customWidth="1"/>
+    <col min="156" max="16384" width="9.109375" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" x14ac:dyDescent="0.25">
@@ -2807,8 +2939,8 @@
     <col min="44" max="44" width="25.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="91" width="9.109375" style="11" customWidth="1"/>
-    <col min="92" max="16384" width="9.109375" style="11"/>
+    <col min="47" max="94" width="9.109375" style="11" customWidth="1"/>
+    <col min="95" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="5" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,8 +3252,8 @@
     <col min="24" max="24" width="24.6640625" style="49" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.44140625" style="49" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.33203125" style="49" bestFit="1" customWidth="1"/>
-    <col min="27" max="60" width="8.88671875" style="49" customWidth="1"/>
-    <col min="61" max="16384" width="8.88671875" style="49"/>
+    <col min="27" max="63" width="8.88671875" style="49" customWidth="1"/>
+    <col min="64" max="16384" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="47" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3346,8 +3478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3381,8 +3513,8 @@
     <col min="30" max="30" width="16.109375" style="53" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="20.33203125" style="53" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="28.109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="33" max="51" width="10.44140625" style="53" customWidth="1"/>
-    <col min="52" max="16384" width="10.44140625" style="53"/>
+    <col min="33" max="54" width="10.44140625" style="53" customWidth="1"/>
+    <col min="55" max="16384" width="10.44140625" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
@@ -3578,7 +3710,7 @@
         <v>332</v>
       </c>
       <c r="AF2" s="82" t="s">
-        <v>424</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -3586,13 +3718,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>222</v>
@@ -3621,7 +3753,7 @@
       <c r="U3" s="84"/>
       <c r="V3" s="84"/>
       <c r="W3" s="62" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="X3" s="53">
         <v>2</v>
@@ -3632,10 +3764,10 @@
       <c r="AB3" s="84"/>
       <c r="AC3" s="84"/>
       <c r="AD3" s="83" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AE3" s="83" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AF3" s="83" t="s">
         <v>227</v>
@@ -3685,8 +3817,8 @@
     <col min="27" max="27" width="11.109375" style="67" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="23" style="18" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="51" width="9.109375" style="53" customWidth="1"/>
-    <col min="52" max="16384" width="9.109375" style="53"/>
+    <col min="30" max="54" width="9.109375" style="53" customWidth="1"/>
+    <col min="55" max="16384" width="9.109375" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="60" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3703,67 +3835,67 @@
         <v>241</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I1" s="59" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="J1" s="59" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K1" s="59" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L1" s="59" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M1" s="59" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N1" s="59" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O1" s="59" t="s">
         <v>190</v>
       </c>
       <c r="P1" s="59" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Q1" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="S1" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>349</v>
-      </c>
       <c r="U1" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="Y1" s="13" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Z1" s="13" t="s">
         <v>206</v>
@@ -3772,10 +3904,10 @@
         <v>207</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3783,7 +3915,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>217</v>
@@ -3792,10 +3924,10 @@
         <v>279</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F2" s="61" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>284</v>
@@ -3804,19 +3936,19 @@
         <v>131</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L2" s="62" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N2" s="63" t="s">
         <v>283</v>
@@ -3825,7 +3957,7 @@
         <v>128</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Q2" s="22" t="s">
         <v>126</v>
@@ -3834,25 +3966,25 @@
         <v>128</v>
       </c>
       <c r="S2" s="22" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="T2" s="22" t="s">
         <v>126</v>
       </c>
       <c r="U2" s="62" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="V2" s="64" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="W2" s="64" t="s">
         <v>226</v>
       </c>
       <c r="X2" s="63" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="Y2" s="63" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Z2" s="64" t="s">
         <v>226</v>
@@ -3864,7 +3996,7 @@
         <v>138</v>
       </c>
       <c r="AC2" s="63" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -3916,31 +4048,31 @@
         <v>241</v>
       </c>
       <c r="F1" s="68" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I1" s="68" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K1" s="68" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3948,7 +4080,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>217</v>
@@ -3963,28 +4095,28 @@
         <v>330</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H2" s="39" t="s">
         <v>330</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>331</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>330</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -3996,8 +4128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4050,43 +4182,43 @@
         <v>241</v>
       </c>
       <c r="E1" s="70" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>290</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="R1" s="71" t="s">
         <v>291</v>
@@ -4095,49 +4227,49 @@
         <v>292</v>
       </c>
       <c r="T1" s="71" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="U1" s="71" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="W1" s="71" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="X1" s="71" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Y1" s="71" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="Z1" s="71" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AA1" s="71" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AB1" s="71" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AC1" s="71" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AD1" s="71" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AE1" s="71" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AF1" s="71" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AG1" s="71" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AH1" s="14" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AI1" s="60"/>
       <c r="AJ1" s="60"/>
@@ -4161,7 +4293,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>217</v>
@@ -4170,7 +4302,7 @@
         <v>279</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>133</v>
@@ -4194,19 +4326,19 @@
         <v>282</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="N2" s="20" t="s">
         <v>138</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="P2" s="73" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="Q2" s="73" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="R2" s="20" t="s">
         <v>151</v>
@@ -4215,13 +4347,13 @@
         <v>151</v>
       </c>
       <c r="T2" s="77" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="U2" s="20" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="W2" s="75"/>
       <c r="X2" s="75"/>
@@ -4232,25 +4364,25 @@
         <v>281</v>
       </c>
       <c r="AA2" s="22" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AB2" s="22" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AC2" s="76" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AD2" s="76" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AE2" s="77" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AF2" s="77" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG2" s="77" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH2" s="77" t="s">
         <v>146</v>
@@ -4276,4 +4408,215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" style="49" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.21875" style="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="86" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>425</v>
+      </c>
+      <c r="E1" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="86" t="s">
+        <v>387</v>
+      </c>
+      <c r="G1" s="86" t="s">
+        <v>426</v>
+      </c>
+      <c r="H1" s="86" t="s">
+        <v>427</v>
+      </c>
+      <c r="I1" s="87" t="s">
+        <v>428</v>
+      </c>
+      <c r="J1" s="88" t="s">
+        <v>388</v>
+      </c>
+      <c r="K1" s="87" t="s">
+        <v>429</v>
+      </c>
+      <c r="L1" s="87" t="s">
+        <v>391</v>
+      </c>
+      <c r="M1" s="87" t="s">
+        <v>430</v>
+      </c>
+      <c r="N1" s="85" t="s">
+        <v>431</v>
+      </c>
+      <c r="O1" s="85" t="s">
+        <v>432</v>
+      </c>
+      <c r="P1" s="85" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q1" s="85" t="s">
+        <v>433</v>
+      </c>
+      <c r="R1" s="71" t="s">
+        <v>400</v>
+      </c>
+      <c r="S1" s="85" t="s">
+        <v>434</v>
+      </c>
+      <c r="T1" s="91" t="s">
+        <v>435</v>
+      </c>
+      <c r="U1" s="91" t="s">
+        <v>436</v>
+      </c>
+      <c r="V1" s="91" t="s">
+        <v>437</v>
+      </c>
+      <c r="W1" s="91" t="s">
+        <v>438</v>
+      </c>
+      <c r="X1" s="91" t="s">
+        <v>439</v>
+      </c>
+      <c r="Y1" s="91" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z1" s="91" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA1" s="91" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB1" s="91" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="89" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="94">
+        <v>2270856920.04</v>
+      </c>
+      <c r="L2" s="94">
+        <v>2270856920.04</v>
+      </c>
+      <c r="M2" s="20"/>
+      <c r="N2" s="89" t="s">
+        <v>446</v>
+      </c>
+      <c r="O2" s="89" t="s">
+        <v>447</v>
+      </c>
+      <c r="P2" s="89" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q2" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="S2" s="90">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="T2" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="92">
+        <v>17871662.100000001</v>
+      </c>
+      <c r="V2" s="93" t="s">
+        <v>449</v>
+      </c>
+      <c r="W2" s="93" t="s">
+        <v>423</v>
+      </c>
+      <c r="X2" s="93" t="s">
+        <v>452</v>
+      </c>
+      <c r="Y2" s="94" t="s">
+        <v>450</v>
+      </c>
+      <c r="Z2" s="94" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA2" s="94" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB2" s="94" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>